<commit_message>
Update ProjectPlan - Sword Boxing.xlsx
</commit_message>
<xml_diff>
--- a/ProjectPlan - Sword Boxing.xlsx
+++ b/ProjectPlan - Sword Boxing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JRizzuto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\College\HU\2024-25\Fall\Game Design 2\SB Github\SwordBoxing_10-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{032C69BA-1A0B-4F50-B446-3C4C870BAFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1334D8CD-385D-4948-9A51-6070207974A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8E3D2AD-8D4D-4882-AC4A-96C7A4B9B379}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B8E3D2AD-8D4D-4882-AC4A-96C7A4B9B379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -95,21 +95,12 @@
     <t>Arena Ring/Stage Modeling</t>
   </si>
   <si>
-    <t>Don't do crowd</t>
-  </si>
-  <si>
     <t>Find reference images</t>
   </si>
   <si>
-    <t>just go online</t>
-  </si>
-  <si>
     <t>Art Director</t>
   </si>
   <si>
-    <t>Producer/Developer</t>
-  </si>
-  <si>
     <t>Narrative Director</t>
   </si>
   <si>
@@ -122,23 +113,200 @@
     <t>Origins/Background Lore</t>
   </si>
   <si>
-    <t>simple, can be expanded on later</t>
-  </si>
-  <si>
     <t>Making the project/refamiliarize with engine</t>
   </si>
   <si>
-    <t>Make Basic 2P Movement</t>
-  </si>
-  <si>
     <t>Use placeholders for now</t>
+  </si>
+  <si>
+    <t>Character modeling for sword fighters</t>
+  </si>
+  <si>
+    <t>Players differentiated by color for now</t>
+  </si>
+  <si>
+    <t>Don't model crowd/audience yet</t>
+  </si>
+  <si>
+    <t>If needed, refer to Joseph for help</t>
+  </si>
+  <si>
+    <t>Simple, can be expanded on later</t>
+  </si>
+  <si>
+    <t>Go online to find these</t>
+  </si>
+  <si>
+    <t>Animations for slice, dodge, punch, and deflect</t>
+  </si>
+  <si>
+    <t>Producer/Sr. Developer</t>
+  </si>
+  <si>
+    <t>Model glove and sword</t>
+  </si>
+  <si>
+    <t>Asset Importation to Unity to replace placeholders</t>
+  </si>
+  <si>
+    <t>Look at photos for reference but can be simple</t>
+  </si>
+  <si>
+    <t>Coordinate with Daniel to implement SFX</t>
+  </si>
+  <si>
+    <t>Finding BGM and cartoonish SFX</t>
+  </si>
+  <si>
+    <t>Make hats and different skin tones for fighter characters</t>
+  </si>
+  <si>
+    <t>Refer to 6.1 in GDD for character design attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Design Stylistics </t>
+  </si>
+  <si>
+    <t>Change colors, size, position, and look of UI in-game</t>
+  </si>
+  <si>
+    <t>Announcer voice lines/dialouge (Session 1)</t>
+  </si>
+  <si>
+    <t>Announcer voice lines/dialouge (Session 2)</t>
+  </si>
+  <si>
+    <t>Refer to 6.2.2 (NPCs) for narration guide</t>
+  </si>
+  <si>
+    <t>Finish most/all of the lines by this date</t>
+  </si>
+  <si>
+    <t>This plan is subject to change.</t>
+  </si>
+  <si>
+    <t>Create interior of arena and locker room (scope: simple)</t>
+  </si>
+  <si>
+    <t>Jr. Developer</t>
+  </si>
+  <si>
+    <t>Brainstorm ideas for assets that can flesh out world</t>
+  </si>
+  <si>
+    <t>Can be things like posters, ads (made-up products), Jumbo-tron, etc.</t>
+  </si>
+  <si>
+    <t>Narrative Director/Jr. Developer</t>
+  </si>
+  <si>
+    <t>Make Basic 2P Controls</t>
+  </si>
+  <si>
+    <t>Health Bars</t>
+  </si>
+  <si>
+    <t>Functionality to lower it to achieve 'win state'</t>
+  </si>
+  <si>
+    <t>Fighting Logic (Session 1)</t>
+  </si>
+  <si>
+    <t>Help Joseph with fighting logic if needed</t>
+  </si>
+  <si>
+    <t>Program when attack moves do damage, stunned state, etc.</t>
+  </si>
+  <si>
+    <t>Implement Placeholder UI (later replaced by Daniel)</t>
+  </si>
+  <si>
+    <t>Split screen functionality (two different cameras)</t>
+  </si>
+  <si>
+    <t>Model low-poly crowd people (people will be copy-pasted in stands)</t>
+  </si>
+  <si>
+    <t>Addendum: Differentiate people in crowd (2-3 different skin tones?)</t>
+  </si>
+  <si>
+    <t>This can be implemented earlier, if applicable</t>
+  </si>
+  <si>
+    <t>Create different scenes for locker room, arena, title screen, etc.</t>
+  </si>
+  <si>
+    <t>Adjust bounds of each scene and add buttons to swap scenes</t>
+  </si>
+  <si>
+    <t>Work with Joseph on this step</t>
+  </si>
+  <si>
+    <t>Work with Peter on this step</t>
+  </si>
+  <si>
+    <t>Items will be attached within engine</t>
+  </si>
+  <si>
+    <t>Touch up title screen UI and other overall UI</t>
+  </si>
+  <si>
+    <t>Fighting Logic (Session 2) and Timer</t>
+  </si>
+  <si>
+    <t>Borrow code from other projects with a timer</t>
+  </si>
+  <si>
+    <t>Incoporate UI Stylistics</t>
+  </si>
+  <si>
+    <t>Specific date TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assist Daniel with asset importation </t>
+  </si>
+  <si>
+    <t>Publish game (??), asset importation</t>
+  </si>
+  <si>
+    <t>Refer to 9.2 GDD for interface assets</t>
+  </si>
+  <si>
+    <t>Use Mixamo if needed, adhere to 9.5 GDD for animation specifications</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Adjust fighting logic, physics, and hitboxes as needed. Balancing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other </t>
+  </si>
+  <si>
+    <t>Help Peter with his Task2</t>
+  </si>
+  <si>
+    <t>Other tasks: TBD</t>
+  </si>
+  <si>
+    <t>Make locker room customization scene (if not already done)</t>
+  </si>
+  <si>
+    <t>Add other narratively driven assets</t>
+  </si>
+  <si>
+    <t>This is up to director's discretion</t>
+  </si>
+  <si>
+    <t>No Task3 this week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +322,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +376,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -201,18 +403,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -234,6 +560,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -553,38 +883,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2020FF7C-A07E-42DC-87EF-C8025935E2C6}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="54.5546875" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="60.44140625" customWidth="1"/>
+    <col min="7" max="7" width="57.77734375" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -593,7 +934,7 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -602,89 +943,104 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="7"/>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -693,7 +1049,7 @@
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -702,32 +1058,104 @@
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -736,7 +1164,7 @@
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -745,32 +1173,120 @@
       <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -779,7 +1295,7 @@
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -788,7 +1304,7 @@
       <c r="G17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -797,23 +1313,109 @@
       <c r="J17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="33" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -822,7 +1424,7 @@
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -831,7 +1433,7 @@
       <c r="G22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -840,11 +1442,336 @@
       <c r="J22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="7"/>
+      <c r="I23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="7"/>
+      <c r="I24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CB6B41D775B04447BD96EAFFE36958CB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d046f2d3fea13a79ac52bb7d41a9fd9f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="058e52c547e1e5289f885b21efdc3561" ns3:_="">
+    <xsd:import namespace="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_activity" ma:index="8" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="14" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF5FD4E0-15A7-44AA-BED1-42CC47AC262A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2025CA95-10B7-4103-A059-18E06315DA7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2564255D-FA8D-4D0F-80AF-2E4959CF7466}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Animation Framework VIII (Extra III)
Additionally:
- Added Lighting
- Sword models are now in characters hands
</commit_message>
<xml_diff>
--- a/ProjectPlan - Sword Boxing.xlsx
+++ b/ProjectPlan - Sword Boxing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\College\HU\2024-25\Fall\Game Design 2\SB Github\SwordBoxing_10-28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8556BDA-413C-4762-AD25-A1B795070A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68ACBB8-533F-4EEC-AD6C-E49D1E606D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B8E3D2AD-8D4D-4882-AC4A-96C7A4B9B379}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -171,16 +171,10 @@
     <t>Program when attack moves do damage, stunned state, etc.</t>
   </si>
   <si>
-    <t>Split screen functionality (two different cameras)</t>
-  </si>
-  <si>
     <t>Create different scenes for locker room, arena, title screen, etc.</t>
   </si>
   <si>
     <t>Items will be attached within engine</t>
-  </si>
-  <si>
-    <t>Borrow code from other projects with a timer</t>
   </si>
   <si>
     <t>Specific date TBD</t>
@@ -230,15 +224,9 @@
     <t>11/18-11/25</t>
   </si>
   <si>
-    <t>Different characters</t>
-  </si>
-  <si>
     <t>Publish game (??), asset importation II</t>
   </si>
   <si>
-    <t>Asset Importation II to replace placeholders</t>
-  </si>
-  <si>
     <t>Asset Importation I, Stamina</t>
   </si>
   <si>
@@ -257,12 +245,6 @@
     <t>Fighting Logic (Session 2)</t>
   </si>
   <si>
-    <t>OPTIONAL</t>
-  </si>
-  <si>
-    <t>Implement Placeholder UI</t>
-  </si>
-  <si>
     <t>Asset importation II (assist others as needed)</t>
   </si>
   <si>
@@ -297,6 +279,15 @@
   </si>
   <si>
     <t>Art/Creative Director</t>
+  </si>
+  <si>
+    <t>Implement UI and Scene Navigation</t>
+  </si>
+  <si>
+    <t>Asset Importation II to replace last placeholders</t>
+  </si>
+  <si>
+    <t>Find different character models</t>
   </si>
 </sst>
 </file>
@@ -491,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -535,9 +526,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -547,8 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -894,7 +881,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,13 +889,13 @@
     <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="60.44140625" customWidth="1"/>
-    <col min="4" max="4" width="44.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="60.44140625" customWidth="1"/>
-    <col min="7" max="7" width="70.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.88671875" customWidth="1"/>
-    <col min="9" max="9" width="51.5546875" customWidth="1"/>
-    <col min="10" max="10" width="52" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="60.109375" customWidth="1"/>
+    <col min="7" max="7" width="67.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+    <col min="9" max="9" width="50.21875" customWidth="1"/>
+    <col min="10" max="10" width="29.5546875" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -955,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="6"/>
@@ -993,7 +980,6 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35"/>
       <c r="E4" s="30"/>
       <c r="F4" t="s">
         <v>42</v>
@@ -1009,7 +995,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -1070,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="6"/>
@@ -1082,14 +1068,13 @@
       <c r="B8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>80</v>
+      <c r="E8" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="F8" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="33"/>
+      <c r="H8" s="32"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1133,9 +1118,9 @@
         <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="32"/>
+        <v>55</v>
+      </c>
+      <c r="H10" s="31"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1197,8 +1182,14 @@
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>80</v>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>74</v>
       </c>
       <c r="F13" t="s">
         <v>39</v>
@@ -1206,12 +1197,14 @@
       <c r="G13" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="34" t="s">
+        <v>74</v>
+      </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K13" s="30"/>
     </row>
@@ -1223,15 +1216,10 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="33"/>
+        <v>64</v>
+      </c>
+      <c r="E14" s="32"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1242,15 +1230,13 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="30"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1258,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1313,21 +1299,19 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="35"/>
-      <c r="K18" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="30"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
@@ -1337,20 +1321,17 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>56</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E19" s="30"/>
       <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>54</v>
       </c>
       <c r="K19" s="7"/>
     </row>
@@ -1359,23 +1340,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>56</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E20" s="30"/>
       <c r="F20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>56</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H20" s="31"/>
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -1438,21 +1415,21 @@
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>71</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K23" s="7"/>
     </row>
@@ -1464,19 +1441,20 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>54</v>
+      </c>
       <c r="F24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="35"/>
+        <v>70</v>
+      </c>
       <c r="H24" s="7"/>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K24" s="7"/>
     </row>
@@ -1488,21 +1466,21 @@
         <v>20</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="12" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>30</v>
@@ -1521,23 +1499,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CB6B41D775B04447BD96EAFFE36958CB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d046f2d3fea13a79ac52bb7d41a9fd9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="058e52c547e1e5289f885b21efdc3561" ns3:_="">
     <xsd:import namespace="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
@@ -1719,31 +1680,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2564255D-FA8D-4D0F-80AF-2E4959CF7466}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2025CA95-10B7-4103-A059-18E06315DA7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF5FD4E0-15A7-44AA-BED1-42CC47AC262A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1759,4 +1713,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2025CA95-10B7-4103-A059-18E06315DA7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2564255D-FA8D-4D0F-80AF-2E4959CF7466}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e862bbfe-0675-4bd0-bfd9-2c99dadd23b8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>